<commit_message>
New MCTS wrapper results and many small Javadoc improvements
- bug fix for ConfigWrapper.EPS (docu & results): use -1e-8 and not -1.
- many small Javadoc enhancements
- extended MCTSWrapperAgentTest (multiple runs, more C4-tests)
- a number of files with MCTS wrapper results on C4, Othello and RubiksCube
</commit_message>
<xml_diff>
--- a/agents/Othello/csv/multiCompeteOthello-i10000-V2.xlsx
+++ b/agents/Othello/csv/multiCompeteOthello-i10000-V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20369"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolfgang\Documents\GitHub\GBG\agents\Othello\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9B0008-6F2B-4C93-80EB-781BBA97CD3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EDD952-2E97-45E2-BF64-C1020EB43BBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="multiCompeteOthello" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">multiCompeteOthello!$A$3:$J$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">multiCompeteOthello!$A$3:$J$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -542,7 +542,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -901,11 +903,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,8 +922,8 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <f>SUBTOTAL(1,H4:H57)</f>
-        <v>0.76666666666666661</v>
+        <f>SUBTOTAL(1,H4:H75)</f>
+        <v>0.76111111111111096</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1084,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1116,7 +1118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1276,7 +1278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1308,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1468,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1500,7 +1502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1660,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -1692,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1852,7 +1854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
@@ -1884,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
@@ -2044,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0</v>
       </c>
@@ -2076,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0</v>
       </c>
@@ -2236,7 +2238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>0</v>
       </c>
@@ -2268,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>0</v>
       </c>
@@ -2428,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>0</v>
       </c>
@@ -2460,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>0</v>
       </c>
@@ -2620,7 +2622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>0</v>
       </c>
@@ -2652,7 +2654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>0</v>
       </c>
@@ -2684,11 +2686,587 @@
         <v>0</v>
       </c>
     </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>0</v>
+      </c>
+      <c r="B58" s="2">
+        <v>10</v>
+      </c>
+      <c r="C58" s="2">
+        <v>1</v>
+      </c>
+      <c r="D58" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E58" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2">
+        <v>1</v>
+      </c>
+      <c r="H58" s="2">
+        <v>1</v>
+      </c>
+      <c r="I58" s="2">
+        <v>0</v>
+      </c>
+      <c r="J58" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>0</v>
+      </c>
+      <c r="B59" s="2">
+        <v>10</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1</v>
+      </c>
+      <c r="D59" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E59" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F59" s="2">
+        <v>1</v>
+      </c>
+      <c r="G59" s="2">
+        <v>1</v>
+      </c>
+      <c r="H59" s="2">
+        <v>1</v>
+      </c>
+      <c r="I59" s="2">
+        <v>0</v>
+      </c>
+      <c r="J59" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>0</v>
+      </c>
+      <c r="B60" s="2">
+        <v>10</v>
+      </c>
+      <c r="C60" s="2">
+        <v>2</v>
+      </c>
+      <c r="D60" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E60" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F60" s="2">
+        <v>0</v>
+      </c>
+      <c r="G60" s="2">
+        <v>1</v>
+      </c>
+      <c r="H60" s="2">
+        <v>1</v>
+      </c>
+      <c r="I60" s="2">
+        <v>0</v>
+      </c>
+      <c r="J60" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>0</v>
+      </c>
+      <c r="B61" s="2">
+        <v>10</v>
+      </c>
+      <c r="C61" s="2">
+        <v>2</v>
+      </c>
+      <c r="D61" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E61" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F61" s="2">
+        <v>1</v>
+      </c>
+      <c r="G61" s="2">
+        <v>1</v>
+      </c>
+      <c r="H61" s="2">
+        <v>1</v>
+      </c>
+      <c r="I61" s="2">
+        <v>0</v>
+      </c>
+      <c r="J61" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>0</v>
+      </c>
+      <c r="B62" s="2">
+        <v>10</v>
+      </c>
+      <c r="C62" s="2">
+        <v>3</v>
+      </c>
+      <c r="D62" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E62" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F62" s="2">
+        <v>0</v>
+      </c>
+      <c r="G62" s="2">
+        <v>1</v>
+      </c>
+      <c r="H62" s="2">
+        <v>1</v>
+      </c>
+      <c r="I62" s="2">
+        <v>0</v>
+      </c>
+      <c r="J62" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>0</v>
+      </c>
+      <c r="B63" s="2">
+        <v>10</v>
+      </c>
+      <c r="C63" s="2">
+        <v>3</v>
+      </c>
+      <c r="D63" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E63" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F63" s="2">
+        <v>1</v>
+      </c>
+      <c r="G63" s="2">
+        <v>1</v>
+      </c>
+      <c r="H63" s="2">
+        <v>1</v>
+      </c>
+      <c r="I63" s="2">
+        <v>0</v>
+      </c>
+      <c r="J63" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>0</v>
+      </c>
+      <c r="B64" s="2">
+        <v>10</v>
+      </c>
+      <c r="C64" s="2">
+        <v>4</v>
+      </c>
+      <c r="D64" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E64" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F64" s="2">
+        <v>0</v>
+      </c>
+      <c r="G64" s="2">
+        <v>1</v>
+      </c>
+      <c r="H64" s="2">
+        <v>1</v>
+      </c>
+      <c r="I64" s="2">
+        <v>0</v>
+      </c>
+      <c r="J64" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>0</v>
+      </c>
+      <c r="B65" s="2">
+        <v>10</v>
+      </c>
+      <c r="C65" s="2">
+        <v>4</v>
+      </c>
+      <c r="D65" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E65" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F65" s="2">
+        <v>1</v>
+      </c>
+      <c r="G65" s="2">
+        <v>1</v>
+      </c>
+      <c r="H65" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I65" s="2">
+        <v>0</v>
+      </c>
+      <c r="J65" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>0</v>
+      </c>
+      <c r="B66" s="2">
+        <v>10</v>
+      </c>
+      <c r="C66" s="2">
+        <v>5</v>
+      </c>
+      <c r="D66" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E66" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F66" s="2">
+        <v>0</v>
+      </c>
+      <c r="G66" s="2">
+        <v>1</v>
+      </c>
+      <c r="H66" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="I66" s="2">
+        <v>0</v>
+      </c>
+      <c r="J66" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>0</v>
+      </c>
+      <c r="B67" s="2">
+        <v>10</v>
+      </c>
+      <c r="C67" s="2">
+        <v>5</v>
+      </c>
+      <c r="D67" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E67" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F67" s="2">
+        <v>1</v>
+      </c>
+      <c r="G67" s="2">
+        <v>1</v>
+      </c>
+      <c r="H67" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I67" s="2">
+        <v>0</v>
+      </c>
+      <c r="J67" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>0</v>
+      </c>
+      <c r="B68" s="2">
+        <v>10</v>
+      </c>
+      <c r="C68" s="2">
+        <v>6</v>
+      </c>
+      <c r="D68" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E68" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F68" s="2">
+        <v>0</v>
+      </c>
+      <c r="G68" s="2">
+        <v>1</v>
+      </c>
+      <c r="H68" s="2">
+        <v>1</v>
+      </c>
+      <c r="I68" s="2">
+        <v>0</v>
+      </c>
+      <c r="J68" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>0</v>
+      </c>
+      <c r="B69" s="2">
+        <v>10</v>
+      </c>
+      <c r="C69" s="2">
+        <v>6</v>
+      </c>
+      <c r="D69" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E69" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F69" s="2">
+        <v>1</v>
+      </c>
+      <c r="G69" s="2">
+        <v>1</v>
+      </c>
+      <c r="H69" s="2">
+        <v>1</v>
+      </c>
+      <c r="I69" s="2">
+        <v>0</v>
+      </c>
+      <c r="J69" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>0</v>
+      </c>
+      <c r="B70" s="2">
+        <v>10</v>
+      </c>
+      <c r="C70" s="2">
+        <v>7</v>
+      </c>
+      <c r="D70" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E70" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F70" s="2">
+        <v>0</v>
+      </c>
+      <c r="G70" s="2">
+        <v>1</v>
+      </c>
+      <c r="H70" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="I70" s="2">
+        <v>0</v>
+      </c>
+      <c r="J70" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>0</v>
+      </c>
+      <c r="B71" s="2">
+        <v>10</v>
+      </c>
+      <c r="C71" s="2">
+        <v>7</v>
+      </c>
+      <c r="D71" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E71" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F71" s="2">
+        <v>1</v>
+      </c>
+      <c r="G71" s="2">
+        <v>1</v>
+      </c>
+      <c r="H71" s="2">
+        <v>0.89999999999999902</v>
+      </c>
+      <c r="I71" s="2">
+        <v>0</v>
+      </c>
+      <c r="J71" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>0</v>
+      </c>
+      <c r="B72" s="2">
+        <v>10</v>
+      </c>
+      <c r="C72" s="2">
+        <v>8</v>
+      </c>
+      <c r="D72" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E72" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F72" s="2">
+        <v>0</v>
+      </c>
+      <c r="G72" s="2">
+        <v>1</v>
+      </c>
+      <c r="H72" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="I72" s="2">
+        <v>0</v>
+      </c>
+      <c r="J72" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>0</v>
+      </c>
+      <c r="B73" s="2">
+        <v>10</v>
+      </c>
+      <c r="C73" s="2">
+        <v>8</v>
+      </c>
+      <c r="D73" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E73" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F73" s="2">
+        <v>1</v>
+      </c>
+      <c r="G73" s="2">
+        <v>1</v>
+      </c>
+      <c r="H73" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="I73" s="2">
+        <v>0</v>
+      </c>
+      <c r="J73" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>0</v>
+      </c>
+      <c r="B74" s="2">
+        <v>10</v>
+      </c>
+      <c r="C74" s="2">
+        <v>9</v>
+      </c>
+      <c r="D74" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E74" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F74" s="2">
+        <v>0</v>
+      </c>
+      <c r="G74" s="2">
+        <v>1</v>
+      </c>
+      <c r="H74" s="3">
+        <v>5.5511151231257802E-17</v>
+      </c>
+      <c r="I74" s="2">
+        <v>0</v>
+      </c>
+      <c r="J74" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>0</v>
+      </c>
+      <c r="B75" s="2">
+        <v>10</v>
+      </c>
+      <c r="C75" s="2">
+        <v>9</v>
+      </c>
+      <c r="D75" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E75" s="3">
+        <v>-1E-8</v>
+      </c>
+      <c r="F75" s="2">
+        <v>1</v>
+      </c>
+      <c r="G75" s="2">
+        <v>1</v>
+      </c>
+      <c r="H75" s="3">
+        <v>5.5511151231257802E-17</v>
+      </c>
+      <c r="I75" s="2">
+        <v>0</v>
+      </c>
+      <c r="J75" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A3:J57" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A3:J75" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="4">
       <filters>
-        <filter val="-1"/>
+        <filter val="-1.00E-08"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>